<commit_message>
T1A - equações corretas
</commit_message>
<xml_diff>
--- a/t1a - snell.xlsx
+++ b/t1a - snell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41442DA4-6439-4DB4-B2D2-3089BF2745B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FAD805-3B6C-4917-8A7E-ACB21DCDDB8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FB603AAF-03AE-4A56-BE8E-5B256B97D4E4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{FB603AAF-03AE-4A56-BE8E-5B256B97D4E4}"/>
   </bookViews>
   <sheets>
     <sheet name="M1-Branco-Plana" sheetId="2" r:id="rId1"/>
@@ -714,6 +714,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -721,9 +724,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -889,12 +889,11 @@
           </c:trendline>
           <c:trendline>
             <c:spPr>
-              <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="19050" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:miter lim="800000"/>
+                <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -904,8 +903,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.5641102636478288E-2"/>
-                  <c:y val="-1.0935017917174628E-3"/>
+                  <c:x val="-5.3876780452301001E-2"/>
+                  <c:y val="-9.7092646699997436E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -932,7 +931,7 @@
                           <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t>y = 0,6556x + 0,338</a:t>
+                      <a:t>y = 0,6847x - 0,0041</a:t>
                     </a:r>
                     <a:endParaRPr lang="en-US">
                       <a:solidFill>
@@ -1932,10 +1931,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:legendEntry>
-        <c:idx val="3"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
@@ -4571,12 +4566,534 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Vermelho-Plana'!$G$3:$G$18</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="16"/>
+                  <c:pt idx="0">
+                    <c:v>8.7103693055957387E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.6705501183531822E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.606965555918767E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.4855283291473127E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8.3672806532745243E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8.2260988427336566E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8.0477216603701673E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7.8928601123914727E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.7229740565879987E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>7.5191328904495522E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>7.3187813751092326E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>7.1484501236426601E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.0630073287338617E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.9907381627290919E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Vermelho-Plana'!$G$3:$G$18</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="16"/>
+                  <c:pt idx="0">
+                    <c:v>8.7103693055957387E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.6705501183531822E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.606965555918767E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.4855283291473127E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8.3672806532745243E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>8.2260988427336566E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8.0477216603701673E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7.8928601123914727E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.7229740565879987E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>7.5191328904495522E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>7.3187813751092326E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>7.1484501236426601E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.0630073287338617E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.9907381627290919E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Vermelho-Plana'!$E$3:$E$18</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="16"/>
+                  <c:pt idx="0">
+                    <c:v>8.6934387363059168E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.5940688946150676E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.4292929993955209E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.2003650947043028E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.9090274601265626E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.5574973509759079E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7.1484501236426601E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6.6849988745162929E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.1706707474421755E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>5.6093800900271539E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>5.0053986630907224E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>4.3633231299858247E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.9846888045879146E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.5153662201880106E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Vermelho-Plana'!$E$3:$E$18</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="16"/>
+                  <c:pt idx="0">
+                    <c:v>8.6934387363059168E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.5940688946150676E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.4292929993955209E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>8.2003650947043028E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>7.9090274601265626E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.5574973509759079E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7.1484501236426601E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>6.6849988745162929E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>6.1706707474421755E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>5.6093800900271539E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>5.0053986630907224E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>4.3633231299858247E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.9846888045879146E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.5153662201880106E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Vermelho-Plana'!$D$3:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>8.7155742747658166E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17364817766693033</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25881904510252074</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34202014332566871</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42261826174069944</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.49999999999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57357643635104605</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.64278760968653925</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.70710678118654746</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.76604444311897801</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8191520442889918</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.8660254037844386</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.93969262078590832</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98480775301220802</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Vermelho-Plana'!$F$3:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>6.1048539534856873E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11320321376790672</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.16504760586067763</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23344536385590539</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28401534470392265</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3338068592337709</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38671096163682062</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.42656873990145833</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.46561452032511141</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.50753836296070409</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.54463903501502708</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.57357643635104605</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.61566147532565818</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.64944804833018366</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E67E-4CA3-8B27-5959788E05CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>+sy</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="6350" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Vermelho-Plana'!$D$3:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>8.7155742747658166E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.17364817766693033</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25881904510252074</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.34202014332566871</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.42261826174069944</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.49999999999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57357643635104605</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.64278760968653925</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.70710678118654746</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.76604444311897801</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.8191520442889918</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.8660254037844386</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.93969262078590832</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.98480775301220802</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Vermelho-Plana'!$G$24:$G$39</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>6.4547593035334389E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12145869200021733</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17750021366712293</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.23224564821737004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28527834983783412</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.33619470764716258</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38460721741828918</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.43014743071958295</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.47246875902988844</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.51124911148644736</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.54619334619084858</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.57703551641708539</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.62550775888720678</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65519303433749498</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.2000445994579356E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.2000445994579356E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E67E-4CA3-8B27-5959788E05CF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>-sy</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="6350" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.5641102636478288E-2"/>
-                  <c:y val="-1.0935017917174628E-3"/>
+                  <c:x val="-3.5322965482026583E-2"/>
+                  <c:y val="-1.8374407702624773E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -4603,7 +5120,7 @@
                           <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t>y = 0,6556x + 0,338</a:t>
+                      <a:t>y = 0,658x - 0,0013</a:t>
                     </a:r>
                     <a:endParaRPr lang="en-US">
                       <a:solidFill>
@@ -4643,514 +5160,6 @@
               </c:txPr>
             </c:trendlineLbl>
           </c:trendline>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'Vermelho-Plana'!$G$3:$G$18</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="16"/>
-                  <c:pt idx="0">
-                    <c:v>8.7103693055957387E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>8.6705501183531822E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>8.606965555918767E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>8.4855283291473127E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>8.3672806532745243E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>8.2260988427336566E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>8.0477216603701673E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>7.8928601123914727E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>7.7229740565879987E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>7.5191328904495522E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>7.3187813751092326E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>7.1484501236426601E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>2.0630073287338617E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>1.9907381627290919E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'Vermelho-Plana'!$G$3:$G$18</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="16"/>
-                  <c:pt idx="0">
-                    <c:v>8.7103693055957387E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>8.6705501183531822E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>8.606965555918767E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>8.4855283291473127E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>8.3672806532745243E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>8.2260988427336566E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>8.0477216603701673E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>7.8928601123914727E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>7.7229740565879987E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>7.5191328904495522E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>7.3187813751092326E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>7.1484501236426601E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>2.0630073287338617E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>1.9907381627290919E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:errBars>
-            <c:errDir val="x"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'Vermelho-Plana'!$E$3:$E$18</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="16"/>
-                  <c:pt idx="0">
-                    <c:v>8.6934387363059168E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>8.5940688946150676E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>8.4292929993955209E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>8.2003650947043028E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>7.9090274601265626E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>7.5574973509759079E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>7.1484501236426601E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>6.6849988745162929E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>6.1706707474421755E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>5.6093800900271539E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>5.0053986630907224E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>4.3633231299858247E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>2.9846888045879146E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>1.5153662201880106E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'Vermelho-Plana'!$E$3:$E$18</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="16"/>
-                  <c:pt idx="0">
-                    <c:v>8.6934387363059168E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>8.5940688946150676E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>8.4292929993955209E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>8.2003650947043028E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>7.9090274601265626E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>7.5574973509759079E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>7.1484501236426601E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>6.6849988745162929E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>6.1706707474421755E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>5.6093800900271539E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>5.0053986630907224E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>4.3633231299858247E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>2.9846888045879146E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>1.5153662201880106E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Vermelho-Plana'!$D$3:$D$18</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>8.7155742747658166E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.17364817766693033</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.25881904510252074</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.34202014332566871</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.42261826174069944</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.49999999999999994</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.57357643635104605</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.64278760968653925</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.70710678118654746</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.76604444311897801</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.8191520442889918</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.8660254037844386</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.93969262078590832</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.98480775301220802</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Vermelho-Plana'!$F$3:$F$18</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>6.1048539534856873E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.11320321376790672</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.16504760586067763</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.23344536385590539</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.28401534470392265</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.3338068592337709</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.38671096163682062</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.42656873990145833</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.46561452032511141</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.50753836296070409</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.54463903501502708</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.57357643635104605</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.61566147532565818</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.64944804833018366</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E67E-4CA3-8B27-5959788E05CF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>+sy</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="6350" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Vermelho-Plana'!$D$3:$D$18</c:f>
-              <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>8.7155742747658166E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.17364817766693033</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.25881904510252074</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.34202014332566871</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.42261826174069944</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.49999999999999994</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.57357643635104605</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.64278760968653925</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.70710678118654746</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.76604444311897801</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.8191520442889918</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.8660254037844386</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.93969262078590832</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.98480775301220802</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Vermelho-Plana'!$G$24:$G$39</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>6.4547593035334389E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.12145869200021733</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.17750021366712293</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.23224564821737004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.28527834983783412</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.33619470764716258</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.38460721741828918</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.43014743071958295</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.47246875902988844</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.51124911148644736</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.54619334619084858</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.57703551641708539</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.62550775888720678</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.65519303433749498</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7.2000445994579356E-3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>7.2000445994579356E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-E67E-4CA3-8B27-5959788E05CF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>-sy</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="6350" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>'Vermelho-Plana'!$D$3:$D$18</c:f>
@@ -10596,12 +10605,11 @@
           </c:trendline>
           <c:trendline>
             <c:spPr>
-              <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+              <a:ln w="19050" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:miter lim="800000"/>
+                <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -10611,8 +10619,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.5641102636478288E-2"/>
-                  <c:y val="-1.0935017917174628E-3"/>
+                  <c:x val="-4.1245311505593123E-2"/>
+                  <c:y val="-1.4098535954498153E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -10639,7 +10647,7 @@
                           <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t>y = 0,6556x + 0,338</a:t>
+                      <a:t>y = 0,6889x - 0,0143</a:t>
                     </a:r>
                     <a:endParaRPr lang="en-US">
                       <a:solidFill>
@@ -11639,10 +11647,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:legendEntry>
-        <c:idx val="3"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
@@ -14290,12 +14294,26 @@
             </c:spPr>
             <c:trendlineType val="linear"/>
             <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.5641102636478288E-2"/>
-                  <c:y val="-1.0935017917174628E-3"/>
+                  <c:x val="-4.6271379077272599E-2"/>
+                  <c:y val="-5.3200000967712612E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -14322,7 +14340,7 @@
                           <a:schemeClr val="accent1"/>
                         </a:solidFill>
                       </a:rPr>
-                      <a:t>y = 0,6556x + 0,338</a:t>
+                      <a:t>y = 0,6828x - 0,0078</a:t>
                     </a:r>
                     <a:endParaRPr lang="en-US">
                       <a:solidFill>
@@ -25196,8 +25214,8 @@
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25214,21 +25232,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="21" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -25532,7 +25550,7 @@
       <c r="A11" s="5">
         <v>45</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="21">
         <v>28.5</v>
       </c>
       <c r="C11" s="5">
@@ -26103,15 +26121,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -26383,12 +26401,12 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
       <c r="I13" s="9" t="s">
         <v>31</v>
       </c>
@@ -26692,7 +26710,7 @@
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
@@ -26710,21 +26728,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="21" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -27599,15 +27617,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -27915,12 +27933,12 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
       <c r="I14" s="7" t="s">
         <v>32</v>
       </c>
@@ -28214,8 +28232,8 @@
   </sheetPr>
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28232,21 +28250,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="21" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -28550,7 +28568,7 @@
       <c r="A11" s="5">
         <v>45</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="21">
         <v>28.5</v>
       </c>
       <c r="C11" s="5">
@@ -29031,15 +29049,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -29347,12 +29365,12 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
       <c r="I14" s="7" t="s">
         <v>32</v>
       </c>
@@ -29646,8 +29664,8 @@
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29664,21 +29682,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="21" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -29982,7 +30000,7 @@
       <c r="A11" s="5">
         <v>45</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="21">
         <v>27.75</v>
       </c>
       <c r="C11" s="5">
@@ -30499,15 +30517,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -30815,12 +30833,12 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
       <c r="I14" s="7" t="s">
         <v>32</v>
       </c>
@@ -31108,9 +31126,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -31260,26 +31281,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EE7295F-EC5E-43B5-90FB-59A1A459F71F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31035FE3-FFA6-4B27-8A73-A608733C4984}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -31303,9 +31313,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31035FE3-FFA6-4B27-8A73-A608733C4984}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9EE7295F-EC5E-43B5-90FB-59A1A459F71F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="c5de1c3e-7813-4da7-ba52-5366b85aaf02"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>